<commit_message>
GROW-81 chore: celery setting 값 변경
</commit_message>
<xml_diff>
--- a/etc/file/usa_stock_list.xlsx
+++ b/etc/file/usa_stock_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="326">
   <si>
     <t>Symbol</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Invesco QQQ Trust</t>
+  </si>
+  <si>
+    <t>QQQM</t>
+  </si>
+  <si>
+    <t>Invesco NASDAQ-100 ETF</t>
   </si>
   <si>
     <t>DIA</t>
@@ -2303,7 +2309,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3166,7 +3172,7 @@
         <v>6</v>
       </c>
       <c r="D57" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E57" s="3"/>
     </row>
@@ -3511,7 +3517,7 @@
         <v>6</v>
       </c>
       <c r="D80" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E80" s="3"/>
     </row>
@@ -3526,7 +3532,7 @@
         <v>6</v>
       </c>
       <c r="D81" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E81" s="3"/>
     </row>
@@ -3601,7 +3607,7 @@
         <v>6</v>
       </c>
       <c r="D86" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E86" s="3"/>
     </row>
@@ -3631,7 +3637,7 @@
         <v>6</v>
       </c>
       <c r="D88" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E88" s="3"/>
     </row>
@@ -3691,7 +3697,7 @@
         <v>6</v>
       </c>
       <c r="D92" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E92" s="3"/>
     </row>
@@ -3700,7 +3706,7 @@
         <v>189</v>
       </c>
       <c r="B93" t="s" s="4">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C93" t="s" s="4">
         <v>6</v>
@@ -3712,10 +3718,10 @@
     </row>
     <row r="94" ht="13.65" customHeight="1">
       <c r="A94" t="s" s="4">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B94" t="s" s="4">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s" s="4">
         <v>6</v>
@@ -3726,25 +3732,25 @@
       <c r="E94" s="3"/>
     </row>
     <row r="95" ht="13.65" customHeight="1">
-      <c r="A95" t="s" s="5">
+      <c r="A95" t="s" s="4">
         <v>192</v>
       </c>
-      <c r="B95" t="s" s="6">
+      <c r="B95" t="s" s="4">
         <v>193</v>
       </c>
       <c r="C95" t="s" s="4">
         <v>6</v>
       </c>
       <c r="D95" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E95" s="3"/>
     </row>
     <row r="96" ht="13.65" customHeight="1">
-      <c r="A96" t="s" s="7">
+      <c r="A96" t="s" s="5">
         <v>194</v>
       </c>
-      <c r="B96" t="s" s="8">
+      <c r="B96" t="s" s="6">
         <v>195</v>
       </c>
       <c r="C96" t="s" s="4">
@@ -3841,7 +3847,7 @@
         <v>6</v>
       </c>
       <c r="D102" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E102" s="3"/>
     </row>
@@ -3856,7 +3862,7 @@
         <v>6</v>
       </c>
       <c r="D103" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E103" s="3"/>
     </row>
@@ -3871,7 +3877,7 @@
         <v>6</v>
       </c>
       <c r="D104" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E104" s="3"/>
     </row>
@@ -3886,7 +3892,7 @@
         <v>6</v>
       </c>
       <c r="D105" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E105" s="3"/>
     </row>
@@ -3916,7 +3922,7 @@
         <v>6</v>
       </c>
       <c r="D107" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E107" s="3"/>
     </row>
@@ -3991,7 +3997,7 @@
         <v>6</v>
       </c>
       <c r="D112" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E112" s="3"/>
     </row>
@@ -4006,7 +4012,7 @@
         <v>6</v>
       </c>
       <c r="D113" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E113" s="3"/>
     </row>
@@ -4036,7 +4042,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E115" s="3"/>
     </row>
@@ -4066,7 +4072,7 @@
         <v>6</v>
       </c>
       <c r="D117" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E117" s="3"/>
     </row>
@@ -4081,7 +4087,7 @@
         <v>6</v>
       </c>
       <c r="D118" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E118" s="3"/>
     </row>
@@ -4096,7 +4102,7 @@
         <v>6</v>
       </c>
       <c r="D119" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E119" s="3"/>
     </row>
@@ -4171,7 +4177,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E124" s="3"/>
     </row>
@@ -4201,7 +4207,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E126" s="3"/>
     </row>
@@ -4246,7 +4252,7 @@
         <v>6</v>
       </c>
       <c r="D129" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E129" s="3"/>
     </row>
@@ -4276,7 +4282,7 @@
         <v>6</v>
       </c>
       <c r="D131" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E131" s="3"/>
     </row>
@@ -4381,7 +4387,7 @@
         <v>6</v>
       </c>
       <c r="D138" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E138" s="3"/>
     </row>
@@ -4456,7 +4462,7 @@
         <v>6</v>
       </c>
       <c r="D143" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E143" s="3"/>
     </row>
@@ -4471,7 +4477,7 @@
         <v>6</v>
       </c>
       <c r="D144" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E144" s="3"/>
     </row>
@@ -4486,7 +4492,7 @@
         <v>6</v>
       </c>
       <c r="D145" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E145" s="3"/>
     </row>
@@ -4576,7 +4582,7 @@
         <v>6</v>
       </c>
       <c r="D151" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E151" s="3"/>
     </row>
@@ -4666,7 +4672,7 @@
         <v>6</v>
       </c>
       <c r="D157" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E157" s="3"/>
     </row>
@@ -4696,7 +4702,7 @@
         <v>6</v>
       </c>
       <c r="D159" t="s" s="4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E159" s="3"/>
     </row>
@@ -4711,22 +4717,30 @@
         <v>6</v>
       </c>
       <c r="D160" t="s" s="4">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E160" s="3"/>
     </row>
     <row r="161" ht="13.65" customHeight="1">
-      <c r="A161" s="9"/>
-      <c r="B161" s="10"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="12"/>
+      <c r="A161" t="s" s="7">
+        <v>324</v>
+      </c>
+      <c r="B161" t="s" s="8">
+        <v>325</v>
+      </c>
+      <c r="C161" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="D161" t="s" s="4">
+        <v>7</v>
+      </c>
       <c r="E161" s="3"/>
     </row>
     <row r="162" ht="13.65" customHeight="1">
       <c r="A162" s="9"/>
       <c r="B162" s="10"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="13"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="12"/>
       <c r="E162" s="3"/>
     </row>
     <row r="163" ht="13.65" customHeight="1">
@@ -4828,15 +4842,22 @@
       <c r="E176" s="3"/>
     </row>
     <row r="177" ht="13.65" customHeight="1">
-      <c r="A177" s="14"/>
-      <c r="B177" s="15"/>
-      <c r="C177" s="15"/>
-      <c r="D177" s="16"/>
+      <c r="A177" s="9"/>
+      <c r="B177" s="10"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="13"/>
       <c r="E177" s="3"/>
+    </row>
+    <row r="178" ht="13.65" customHeight="1">
+      <c r="A178" s="14"/>
+      <c r="B178" s="15"/>
+      <c r="C178" s="15"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B121" r:id="rId1" location="" tooltip="" display="JD.com"/>
+    <hyperlink ref="B122" r:id="rId1" location="" tooltip="" display="JD.com, Inc."/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>